<commit_message>
Final Notebook from Presentation
</commit_message>
<xml_diff>
--- a/results/model1/model1_df_results.xlsx
+++ b/results/model1/model1_df_results.xlsx
@@ -44,17 +44,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00D4EECE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="008ACE88"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="004DB163"/>
+        <fgColor rgb="00A2D99C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0050B264"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="002A924A"/>
       </patternFill>
     </fill>
     <fill>
@@ -64,17 +64,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0055B567"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="009CD797"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00E0F3DB"/>
+        <fgColor rgb="0046AE60"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0098D594"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00DFF3DA"/>
       </patternFill>
     </fill>
     <fill>
@@ -84,27 +84,27 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0076C578"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="003FA95C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0094D390"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00D5EFCF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00F0F9EC"/>
+        <fgColor rgb="00E7F6E3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="004AAF61"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0029914A"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="009BD696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00DEF2D9"/>
       </patternFill>
     </fill>
   </fills>
@@ -138,40 +138,40 @@
     <xf applyAlignment="1" borderId="0" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf applyAlignment="1" borderId="0" fillId="10" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="11" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="12" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="5" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="6" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="7" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="13" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="8" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="14" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf applyAlignment="1" borderId="0" fillId="9" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="10" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="11" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="5" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="6" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="7" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="12" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="8" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="13" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="14" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -509,13 +509,13 @@
         <v>-4</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>-5.4946</v>
+        <v>-4.8629</v>
       </c>
       <c r="D2" s="3" t="n">
-        <v>0.6951000000000001</v>
+        <v>0.6604</v>
       </c>
       <c r="E2" s="4" t="n">
-        <v>2.2144</v>
+        <v>2.118</v>
       </c>
     </row>
     <row r="3">
@@ -526,13 +526,13 @@
         <v>-3</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>-0.5142</v>
+        <v>-0.4464</v>
       </c>
       <c r="D3" s="5" t="n">
-        <v>0.5109</v>
+        <v>0.4994</v>
       </c>
       <c r="E3" s="6" t="n">
-        <v>1.2155</v>
+        <v>1.2062</v>
       </c>
     </row>
     <row r="4">
@@ -543,13 +543,13 @@
         <v>-2</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>0.4993</v>
+        <v>0.4723</v>
       </c>
       <c r="D4" s="7" t="n">
-        <v>0.3923</v>
+        <v>0.4027</v>
       </c>
       <c r="E4" s="8" t="n">
-        <v>0.9444</v>
+        <v>0.9859</v>
       </c>
     </row>
     <row r="5">
@@ -560,13 +560,13 @@
         <v>-1</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>0.9862</v>
+        <v>0.9219000000000001</v>
       </c>
       <c r="D5" s="9" t="n">
-        <v>0.0814</v>
+        <v>0.1936</v>
       </c>
       <c r="E5" s="9" t="n">
-        <v>0.2002</v>
+        <v>0.4756</v>
       </c>
     </row>
     <row r="6">
@@ -577,13 +577,13 @@
         <v>0</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>0.7265</v>
+        <v>0.6124000000000001</v>
       </c>
       <c r="D6" s="10" t="n">
-        <v>0.4052</v>
-      </c>
-      <c r="E6" s="7" t="n">
-        <v>1.0164</v>
+        <v>0.4823</v>
+      </c>
+      <c r="E6" s="6" t="n">
+        <v>1.2105</v>
       </c>
     </row>
     <row r="7">
@@ -594,13 +594,13 @@
         <v>1</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>0.5006</v>
+        <v>0.3245</v>
       </c>
       <c r="D7" s="11" t="n">
-        <v>0.5497</v>
+        <v>0.6393</v>
       </c>
       <c r="E7" s="12" t="n">
-        <v>1.3832</v>
+        <v>1.5981</v>
       </c>
     </row>
     <row r="8">
@@ -611,13 +611,13 @@
         <v>2</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>0.1375</v>
+        <v>-0.0885</v>
       </c>
       <c r="D8" s="13" t="n">
-        <v>0.7345</v>
+        <v>0.8250999999999999</v>
       </c>
       <c r="E8" s="14" t="n">
-        <v>1.8214</v>
+        <v>2.0341</v>
       </c>
     </row>
     <row r="9">
@@ -628,13 +628,13 @@
         <v>3</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>-0.1031</v>
-      </c>
-      <c r="D9" s="4" t="n">
-        <v>0.847</v>
+        <v>-0.3501</v>
+      </c>
+      <c r="D9" s="15" t="n">
+        <v>0.9371</v>
       </c>
       <c r="E9" s="15" t="n">
-        <v>2.1073</v>
+        <v>2.3226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moved new class to separate ipynb
</commit_message>
<xml_diff>
--- a/results/model1/model1_df_results.xlsx
+++ b/results/model1/model1_df_results.xlsx
@@ -35,7 +35,7 @@
       <color rgb="00F1F1F1"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill/>
     </fill>
@@ -44,17 +44,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00A2D99C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0050B264"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="002A924A"/>
+        <fgColor rgb="00CBEAC4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0080CA80"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="004BB062"/>
       </patternFill>
     </fill>
     <fill>
@@ -64,17 +64,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0046AE60"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0098D594"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00DFF3DA"/>
+        <fgColor rgb="0056B567"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="009ED798"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E1F3DC"/>
       </patternFill>
     </fill>
     <fill>
@@ -84,17 +84,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00E7F6E3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="004AAF61"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0029914A"/>
+        <fgColor rgb="0076C578"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0043AC5E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0055B567"/>
       </patternFill>
     </fill>
     <fill>
@@ -104,7 +104,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00DEF2D9"/>
+        <fgColor rgb="00DBF1D6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F4FBF2"/>
       </patternFill>
     </fill>
   </fills>
@@ -127,7 +132,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -138,27 +143,30 @@
     <xf applyAlignment="1" borderId="0" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf applyAlignment="1" borderId="0" fillId="9" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf applyAlignment="1" borderId="0" fillId="10" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="11" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="5" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="6" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="12" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="5" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="6" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
     <xf applyAlignment="1" borderId="0" fillId="7" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
@@ -171,7 +179,7 @@
     <xf applyAlignment="1" borderId="0" fillId="14" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="9" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="15" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -509,13 +517,13 @@
         <v>-4</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>-4.8629</v>
+        <v>-5.7686</v>
       </c>
       <c r="D2" s="3" t="n">
-        <v>0.6604</v>
+        <v>0.7096</v>
       </c>
       <c r="E2" s="4" t="n">
-        <v>2.118</v>
+        <v>2.2721</v>
       </c>
     </row>
     <row r="3">
@@ -526,13 +534,13 @@
         <v>-3</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>-0.4464</v>
+        <v>-0.5945</v>
       </c>
       <c r="D3" s="5" t="n">
-        <v>0.4994</v>
+        <v>0.5243</v>
       </c>
       <c r="E3" s="6" t="n">
-        <v>1.2062</v>
+        <v>1.2607</v>
       </c>
     </row>
     <row r="4">
@@ -543,13 +551,13 @@
         <v>-2</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>0.4723</v>
+        <v>0.4392</v>
       </c>
       <c r="D4" s="7" t="n">
-        <v>0.4027</v>
+        <v>0.4152</v>
       </c>
       <c r="E4" s="8" t="n">
-        <v>0.9859</v>
+        <v>1.0114</v>
       </c>
     </row>
     <row r="5">
@@ -560,13 +568,13 @@
         <v>-1</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>0.9219000000000001</v>
+        <v>0.9815</v>
       </c>
       <c r="D5" s="9" t="n">
-        <v>0.1936</v>
+        <v>0.09429999999999999</v>
       </c>
       <c r="E5" s="9" t="n">
-        <v>0.4756</v>
+        <v>0.2302</v>
       </c>
     </row>
     <row r="6">
@@ -577,13 +585,13 @@
         <v>0</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>0.6124000000000001</v>
+        <v>0.6804</v>
       </c>
       <c r="D6" s="10" t="n">
-        <v>0.4823</v>
-      </c>
-      <c r="E6" s="6" t="n">
-        <v>1.2105</v>
+        <v>0.438</v>
+      </c>
+      <c r="E6" s="11" t="n">
+        <v>1.0993</v>
       </c>
     </row>
     <row r="7">
@@ -594,13 +602,13 @@
         <v>1</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>0.3245</v>
-      </c>
-      <c r="D7" s="11" t="n">
-        <v>0.6393</v>
-      </c>
-      <c r="E7" s="12" t="n">
-        <v>1.5981</v>
+        <v>0.427</v>
+      </c>
+      <c r="D7" s="12" t="n">
+        <v>0.5888</v>
+      </c>
+      <c r="E7" s="13" t="n">
+        <v>1.4735</v>
       </c>
     </row>
     <row r="8">
@@ -611,13 +619,13 @@
         <v>2</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>-0.0885</v>
-      </c>
-      <c r="D8" s="13" t="n">
-        <v>0.8250999999999999</v>
-      </c>
-      <c r="E8" s="14" t="n">
-        <v>2.0341</v>
+        <v>0.0192</v>
+      </c>
+      <c r="D8" s="14" t="n">
+        <v>0.7832</v>
+      </c>
+      <c r="E8" s="15" t="n">
+        <v>1.9327</v>
       </c>
     </row>
     <row r="9">
@@ -628,13 +636,13 @@
         <v>3</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>-0.3501</v>
-      </c>
-      <c r="D9" s="15" t="n">
-        <v>0.9371</v>
-      </c>
-      <c r="E9" s="15" t="n">
-        <v>2.3226</v>
+        <v>-0.2416</v>
+      </c>
+      <c r="D9" s="4" t="n">
+        <v>0.8987000000000001</v>
+      </c>
+      <c r="E9" s="16" t="n">
+        <v>2.23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
separate nb for laptop
</commit_message>
<xml_diff>
--- a/results/model1/model1_df_results.xlsx
+++ b/results/model1/model1_df_results.xlsx
@@ -44,17 +44,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00CBEAC4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0080CA80"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="004BB062"/>
+        <fgColor rgb="00CAEAC3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0081CA81"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0045AD5F"/>
       </patternFill>
     </fill>
     <fill>
@@ -64,17 +64,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0056B567"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="009ED798"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00E1F3DC"/>
+        <fgColor rgb="0053B466"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="009CD797"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E0F3DB"/>
       </patternFill>
     </fill>
     <fill>
@@ -89,12 +89,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0043AC5E"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0055B567"/>
+        <fgColor rgb="003FA95C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0052B365"/>
       </patternFill>
     </fill>
     <fill>
@@ -104,7 +104,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00DBF1D6"/>
+        <fgColor rgb="00DBF1D5"/>
       </patternFill>
     </fill>
     <fill>
@@ -517,13 +517,13 @@
         <v>-4</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>-5.7686</v>
+        <v>-5.8419</v>
       </c>
       <c r="D2" s="3" t="n">
-        <v>0.7096</v>
+        <v>0.7134</v>
       </c>
       <c r="E2" s="4" t="n">
-        <v>2.2721</v>
+        <v>2.2842</v>
       </c>
     </row>
     <row r="3">
@@ -534,13 +534,13 @@
         <v>-3</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>-0.5945</v>
+        <v>-0.6576</v>
       </c>
       <c r="D3" s="5" t="n">
-        <v>0.5243</v>
+        <v>0.5346</v>
       </c>
       <c r="E3" s="6" t="n">
-        <v>1.2607</v>
+        <v>1.2849</v>
       </c>
     </row>
     <row r="4">
@@ -551,13 +551,13 @@
         <v>-2</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>0.4392</v>
+        <v>0.4411</v>
       </c>
       <c r="D4" s="7" t="n">
-        <v>0.4152</v>
+        <v>0.4145</v>
       </c>
       <c r="E4" s="8" t="n">
-        <v>1.0114</v>
+        <v>1.0097</v>
       </c>
     </row>
     <row r="5">
@@ -568,13 +568,13 @@
         <v>-1</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>0.9815</v>
+        <v>0.9759</v>
       </c>
       <c r="D5" s="9" t="n">
-        <v>0.09429999999999999</v>
+        <v>0.1075</v>
       </c>
       <c r="E5" s="9" t="n">
-        <v>0.2302</v>
+        <v>0.2625</v>
       </c>
     </row>
     <row r="6">
@@ -585,13 +585,13 @@
         <v>0</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>0.6804</v>
+        <v>0.6758999999999999</v>
       </c>
       <c r="D6" s="10" t="n">
-        <v>0.438</v>
+        <v>0.4411</v>
       </c>
       <c r="E6" s="11" t="n">
-        <v>1.0993</v>
+        <v>1.1066</v>
       </c>
     </row>
     <row r="7">
@@ -602,13 +602,13 @@
         <v>1</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>0.427</v>
+        <v>0.416</v>
       </c>
       <c r="D7" s="12" t="n">
-        <v>0.5888</v>
+        <v>0.5944</v>
       </c>
       <c r="E7" s="13" t="n">
-        <v>1.4735</v>
+        <v>1.4866</v>
       </c>
     </row>
     <row r="8">
@@ -619,13 +619,13 @@
         <v>2</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>0.0192</v>
+        <v>0.0075</v>
       </c>
       <c r="D8" s="14" t="n">
-        <v>0.7832</v>
+        <v>0.7879</v>
       </c>
       <c r="E8" s="15" t="n">
-        <v>1.9327</v>
+        <v>1.9432</v>
       </c>
     </row>
     <row r="9">
@@ -636,13 +636,13 @@
         <v>3</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>-0.2416</v>
+        <v>-0.2553</v>
       </c>
       <c r="D9" s="4" t="n">
-        <v>0.8987000000000001</v>
+        <v>0.9036</v>
       </c>
       <c r="E9" s="16" t="n">
-        <v>2.23</v>
+        <v>2.2414</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new README - requires cleaning
</commit_message>
<xml_diff>
--- a/results/model1/model1_df_results.xlsx
+++ b/results/model1/model1_df_results.xlsx
@@ -44,7 +44,47 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0091D28E"/>
+        <fgColor rgb="00F7FCF5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00BBE4B4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0084CC83"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0000441B"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00369F54"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="006ABF71"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00D0EDCA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F1FAEE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0068BE70"/>
       </patternFill>
     </fill>
     <fill>
@@ -54,62 +94,22 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="001A843F"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0000441B"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0043AC5E"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0099D595"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00DFF3DA"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00F7FCF5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00DBF1D6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="003AA357"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0019833E"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0048AE60"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="009CD797"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00DDF2D8"/>
+        <fgColor rgb="00208843"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="003CA559"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="008DD08A"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00B2E0AC"/>
       </patternFill>
     </fill>
   </fills>
@@ -143,43 +143,43 @@
     <xf applyAlignment="1" borderId="0" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf applyAlignment="1" borderId="0" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf applyAlignment="1" borderId="0" fillId="10" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="11" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="12" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
     <xf applyAlignment="1" borderId="0" fillId="5" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="6" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf applyAlignment="1" borderId="0" fillId="12" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="7" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf applyAlignment="1" borderId="0" fillId="13" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="7" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="8" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="14" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="8" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="9" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="15" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="9" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -517,13 +517,13 @@
         <v>-4</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>-4.4159</v>
+        <v>-8.163399999999999</v>
       </c>
       <c r="D2" s="3" t="n">
-        <v>0.6347</v>
-      </c>
-      <c r="E2" s="4" t="n">
-        <v>2.0347</v>
+        <v>0.8256</v>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>2.629</v>
       </c>
     </row>
     <row r="3">
@@ -534,13 +534,13 @@
         <v>-3</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>-0.2963</v>
-      </c>
-      <c r="D3" s="5" t="n">
-        <v>0.4727</v>
-      </c>
-      <c r="E3" s="6" t="n">
-        <v>1.1431</v>
+        <v>-1.5348</v>
+      </c>
+      <c r="D3" s="4" t="n">
+        <v>0.6611</v>
+      </c>
+      <c r="E3" s="5" t="n">
+        <v>1.5656</v>
       </c>
     </row>
     <row r="4">
@@ -551,13 +551,13 @@
         <v>-2</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>0.5569</v>
-      </c>
-      <c r="D4" s="7" t="n">
-        <v>0.3691</v>
-      </c>
-      <c r="E4" s="8" t="n">
-        <v>0.905</v>
+        <v>-0.0432</v>
+      </c>
+      <c r="D4" s="6" t="n">
+        <v>0.5663</v>
+      </c>
+      <c r="E4" s="7" t="n">
+        <v>1.3511</v>
       </c>
     </row>
     <row r="5">
@@ -568,13 +568,13 @@
         <v>-1</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>0.9101</v>
-      </c>
-      <c r="D5" s="9" t="n">
-        <v>0.2078</v>
-      </c>
-      <c r="E5" s="9" t="n">
-        <v>0.5103</v>
+        <v>0.8611</v>
+      </c>
+      <c r="D5" s="8" t="n">
+        <v>0.2582</v>
+      </c>
+      <c r="E5" s="8" t="n">
+        <v>0.6246</v>
       </c>
     </row>
     <row r="6">
@@ -585,13 +585,13 @@
         <v>0</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>0.6037</v>
-      </c>
-      <c r="D6" s="10" t="n">
-        <v>0.4877</v>
-      </c>
-      <c r="E6" s="11" t="n">
-        <v>1.2245</v>
+        <v>0.6677999999999999</v>
+      </c>
+      <c r="D6" s="9" t="n">
+        <v>0.4465</v>
+      </c>
+      <c r="E6" s="10" t="n">
+        <v>1.1071</v>
       </c>
     </row>
     <row r="7">
@@ -602,13 +602,13 @@
         <v>1</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>0.3004</v>
-      </c>
-      <c r="D7" s="12" t="n">
-        <v>0.6506</v>
-      </c>
-      <c r="E7" s="13" t="n">
-        <v>1.6265</v>
+        <v>0.5405</v>
+      </c>
+      <c r="D7" s="11" t="n">
+        <v>0.5273</v>
+      </c>
+      <c r="E7" s="12" t="n">
+        <v>1.3321</v>
       </c>
     </row>
     <row r="8">
@@ -619,13 +619,13 @@
         <v>2</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>-0.1039</v>
-      </c>
-      <c r="D8" s="14" t="n">
-        <v>0.8309</v>
-      </c>
-      <c r="E8" s="15" t="n">
-        <v>2.0484</v>
+        <v>0.2033</v>
+      </c>
+      <c r="D8" s="13" t="n">
+        <v>0.7059</v>
+      </c>
+      <c r="E8" s="14" t="n">
+        <v>1.7616</v>
       </c>
     </row>
     <row r="9">
@@ -636,13 +636,13 @@
         <v>3</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>-0.3651</v>
-      </c>
-      <c r="D9" s="16" t="n">
-        <v>0.9423</v>
+        <v>0.0177</v>
+      </c>
+      <c r="D9" s="15" t="n">
+        <v>0.7993</v>
       </c>
       <c r="E9" s="16" t="n">
-        <v>2.3351</v>
+        <v>1.9911</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating readme and final models
</commit_message>
<xml_diff>
--- a/results/model1/model1_df_results.xlsx
+++ b/results/model1/model1_df_results.xlsx
@@ -44,72 +44,72 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="00AADDA4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0058B668"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00268E47"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0000441B"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0048AE60"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="009CD797"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00DFF3DA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="00F7FCF5"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00BBE4B4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0084CC83"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0000441B"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00369F54"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="006ABF71"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00D0EDCA"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00F1FAEE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0068BE70"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="003EA75A"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00208843"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="003CA559"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="008DD08A"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00B2E0AC"/>
+        <fgColor rgb="00EAF7E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0050B264"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00248C46"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="004BB062"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="009FD899"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00DEF2D9"/>
       </patternFill>
     </fill>
   </fills>
@@ -143,16 +143,19 @@
     <xf applyAlignment="1" borderId="0" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf applyAlignment="1" borderId="0" fillId="10" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf applyAlignment="1" borderId="0" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="10" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="11" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="11" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="12" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="5" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
@@ -161,25 +164,22 @@
     <xf applyAlignment="1" borderId="0" fillId="6" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="12" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="13" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="7" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="13" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="14" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="8" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="14" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="15" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="9" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="15" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -517,13 +517,13 @@
         <v>-4</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>-8.163399999999999</v>
+        <v>-4.8372</v>
       </c>
       <c r="D2" s="3" t="n">
-        <v>0.8256</v>
-      </c>
-      <c r="E2" s="3" t="n">
-        <v>2.629</v>
+        <v>0.659</v>
+      </c>
+      <c r="E2" s="4" t="n">
+        <v>2.1093</v>
       </c>
     </row>
     <row r="3">
@@ -534,13 +534,13 @@
         <v>-3</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>-1.5348</v>
-      </c>
-      <c r="D3" s="4" t="n">
-        <v>0.6611</v>
-      </c>
-      <c r="E3" s="5" t="n">
-        <v>1.5656</v>
+        <v>-0.3791</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <v>0.4876</v>
+      </c>
+      <c r="E3" s="6" t="n">
+        <v>1.1749</v>
       </c>
     </row>
     <row r="4">
@@ -551,13 +551,13 @@
         <v>-2</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>-0.0432</v>
-      </c>
-      <c r="D4" s="6" t="n">
-        <v>0.5663</v>
-      </c>
-      <c r="E4" s="7" t="n">
-        <v>1.3511</v>
+        <v>0.5788</v>
+      </c>
+      <c r="D4" s="7" t="n">
+        <v>0.3598</v>
+      </c>
+      <c r="E4" s="8" t="n">
+        <v>0.8798</v>
       </c>
     </row>
     <row r="5">
@@ -568,13 +568,13 @@
         <v>-1</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>0.8611</v>
-      </c>
-      <c r="D5" s="8" t="n">
-        <v>0.2582</v>
-      </c>
-      <c r="E5" s="8" t="n">
-        <v>0.6246</v>
+        <v>0.9464</v>
+      </c>
+      <c r="D5" s="9" t="n">
+        <v>0.1605</v>
+      </c>
+      <c r="E5" s="9" t="n">
+        <v>0.3939</v>
       </c>
     </row>
     <row r="6">
@@ -585,13 +585,13 @@
         <v>0</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>0.6677999999999999</v>
-      </c>
-      <c r="D6" s="9" t="n">
-        <v>0.4465</v>
-      </c>
-      <c r="E6" s="10" t="n">
-        <v>1.1071</v>
+        <v>0.6488</v>
+      </c>
+      <c r="D6" s="10" t="n">
+        <v>0.4591</v>
+      </c>
+      <c r="E6" s="11" t="n">
+        <v>1.1526</v>
       </c>
     </row>
     <row r="7">
@@ -602,13 +602,13 @@
         <v>1</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>0.5405</v>
-      </c>
-      <c r="D7" s="11" t="n">
-        <v>0.5273</v>
-      </c>
-      <c r="E7" s="12" t="n">
-        <v>1.3321</v>
+        <v>0.3559</v>
+      </c>
+      <c r="D7" s="12" t="n">
+        <v>0.6243</v>
+      </c>
+      <c r="E7" s="13" t="n">
+        <v>1.5611</v>
       </c>
     </row>
     <row r="8">
@@ -619,13 +619,13 @@
         <v>2</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>0.2033</v>
-      </c>
-      <c r="D8" s="13" t="n">
-        <v>0.7059</v>
-      </c>
-      <c r="E8" s="14" t="n">
-        <v>1.7616</v>
+        <v>-0.0419</v>
+      </c>
+      <c r="D8" s="14" t="n">
+        <v>0.8072</v>
+      </c>
+      <c r="E8" s="15" t="n">
+        <v>1.9906</v>
       </c>
     </row>
     <row r="9">
@@ -636,13 +636,13 @@
         <v>3</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>0.0177</v>
-      </c>
-      <c r="D9" s="15" t="n">
-        <v>0.7993</v>
+        <v>-0.3054</v>
+      </c>
+      <c r="D9" s="16" t="n">
+        <v>0.9215</v>
       </c>
       <c r="E9" s="16" t="n">
-        <v>1.9911</v>
+        <v>2.2846</v>
       </c>
     </row>
   </sheetData>

</xml_diff>